<commit_message>
fix: embed id and url
</commit_message>
<xml_diff>
--- a/public/Buscador de indicadores_11_12_2025.xlsx
+++ b/public/Buscador de indicadores_11_12_2025.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduardo.kawanabe\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\juanjo\javascript_projects\buscador-rema\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FCBC922-1358-4775-83FD-0FF69CB7579A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159C74F8-4B4D-4967-94C3-FF6308D9FF39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$F$227</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$I$227</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="710">
   <si>
     <t>Nombre</t>
   </si>
@@ -2157,6 +2157,18 @@
   </si>
   <si>
     <t>title</t>
+  </si>
+  <si>
+    <t>infogram_0__/DkMCTXdkMa8lmqASrpBv</t>
+  </si>
+  <si>
+    <t>https://e.infogram.com/js/dist/embed.js?8VU</t>
+  </si>
+  <si>
+    <t>infogram_0__/dM9lgy3ygZsXO8c9tHVO</t>
+  </si>
+  <si>
+    <t>https://e.infogram.com/js/dist/embed.js?bd7</t>
   </si>
 </sst>
 </file>
@@ -2517,24 +2529,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I227"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="159" style="1" customWidth="1"/>
     <col min="2" max="2" width="29" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="44.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="56.5703125" style="1" customWidth="1"/>
-    <col min="6" max="8" width="80.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="44.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="56.5546875" style="1" customWidth="1"/>
+    <col min="6" max="8" width="80.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2563,7 +2576,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2585,7 +2598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -2601,13 +2614,17 @@
       <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>707</v>
+      </c>
       <c r="I3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -2629,7 +2646,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -2651,7 +2668,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -2673,7 +2690,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -2695,7 +2712,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -2717,7 +2734,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -2739,7 +2756,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
@@ -2761,7 +2778,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -2780,7 +2797,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -2799,7 +2816,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
@@ -2818,7 +2835,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
@@ -2837,7 +2854,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
@@ -2856,7 +2873,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
@@ -2875,7 +2892,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>57</v>
       </c>
@@ -2894,7 +2911,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
@@ -2913,7 +2930,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>63</v>
       </c>
@@ -2932,7 +2949,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>66</v>
       </c>
@@ -2951,7 +2968,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>69</v>
       </c>
@@ -2970,7 +2987,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
@@ -2989,7 +3006,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>75</v>
       </c>
@@ -3008,7 +3025,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>78</v>
       </c>
@@ -3027,7 +3044,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>81</v>
       </c>
@@ -3046,7 +3063,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>84</v>
       </c>
@@ -3065,7 +3082,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>87</v>
       </c>
@@ -3084,7 +3101,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>90</v>
       </c>
@@ -3103,7 +3120,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>93</v>
       </c>
@@ -3122,7 +3139,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>96</v>
       </c>
@@ -3141,7 +3158,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>100</v>
       </c>
@@ -3158,7 +3175,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>103</v>
       </c>
@@ -3175,7 +3192,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>106</v>
       </c>
@@ -3192,7 +3209,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>109</v>
       </c>
@@ -3209,7 +3226,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>112</v>
       </c>
@@ -3226,7 +3243,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>115</v>
       </c>
@@ -3243,7 +3260,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>118</v>
       </c>
@@ -3260,7 +3277,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>121</v>
       </c>
@@ -3277,7 +3294,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>124</v>
       </c>
@@ -3294,7 +3311,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>127</v>
       </c>
@@ -3311,7 +3328,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>130</v>
       </c>
@@ -3328,7 +3345,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>133</v>
       </c>
@@ -3345,7 +3362,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>137</v>
       </c>
@@ -3361,11 +3378,17 @@
       <c r="F43" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="G43" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>709</v>
+      </c>
       <c r="I43" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>141</v>
       </c>
@@ -3385,7 +3408,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>144</v>
       </c>
@@ -3408,7 +3431,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>148</v>
       </c>
@@ -3428,7 +3451,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>152</v>
       </c>
@@ -3451,7 +3474,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>156</v>
       </c>
@@ -3474,7 +3497,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>159</v>
       </c>
@@ -3497,7 +3520,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>162</v>
       </c>
@@ -3520,7 +3543,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>165</v>
       </c>
@@ -3543,7 +3566,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>168</v>
       </c>
@@ -3566,7 +3589,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>171</v>
       </c>
@@ -3586,7 +3609,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>175</v>
       </c>
@@ -3606,7 +3629,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>178</v>
       </c>
@@ -3626,7 +3649,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>181</v>
       </c>
@@ -3646,7 +3669,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>184</v>
       </c>
@@ -3666,7 +3689,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>187</v>
       </c>
@@ -3686,7 +3709,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>191</v>
       </c>
@@ -3706,7 +3729,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>194</v>
       </c>
@@ -3726,7 +3749,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>197</v>
       </c>
@@ -3746,7 +3769,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>200</v>
       </c>
@@ -3766,7 +3789,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>203</v>
       </c>
@@ -3786,7 +3809,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>206</v>
       </c>
@@ -3806,7 +3829,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>209</v>
       </c>
@@ -3826,7 +3849,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>212</v>
       </c>
@@ -3846,7 +3869,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>215</v>
       </c>
@@ -3866,7 +3889,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>220</v>
       </c>
@@ -3886,7 +3909,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>223</v>
       </c>
@@ -3906,7 +3929,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>226</v>
       </c>
@@ -3926,7 +3949,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>229</v>
       </c>
@@ -3946,7 +3969,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>232</v>
       </c>
@@ -3966,7 +3989,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>235</v>
       </c>
@@ -3986,7 +4009,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>238</v>
       </c>
@@ -4006,7 +4029,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>242</v>
       </c>
@@ -4023,7 +4046,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>245</v>
       </c>
@@ -4043,7 +4066,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>249</v>
       </c>
@@ -4060,7 +4083,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>252</v>
       </c>
@@ -4077,7 +4100,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>255</v>
       </c>
@@ -4094,7 +4117,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>258</v>
       </c>
@@ -4111,7 +4134,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>261</v>
       </c>
@@ -4128,7 +4151,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>264</v>
       </c>
@@ -4145,7 +4168,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>267</v>
       </c>
@@ -4162,7 +4185,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>270</v>
       </c>
@@ -4179,7 +4202,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>273</v>
       </c>
@@ -4196,7 +4219,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>276</v>
       </c>
@@ -4213,7 +4236,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>279</v>
       </c>
@@ -4230,7 +4253,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>282</v>
       </c>
@@ -4247,7 +4270,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>285</v>
       </c>
@@ -4264,7 +4287,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>288</v>
       </c>
@@ -4284,7 +4307,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>292</v>
       </c>
@@ -4301,7 +4324,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>295</v>
       </c>
@@ -4318,7 +4341,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>298</v>
       </c>
@@ -4335,7 +4358,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>301</v>
       </c>
@@ -4352,7 +4375,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>304</v>
       </c>
@@ -4369,7 +4392,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>307</v>
       </c>
@@ -4386,7 +4409,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>310</v>
       </c>
@@ -4403,7 +4426,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>313</v>
       </c>
@@ -4420,7 +4443,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>316</v>
       </c>
@@ -4440,7 +4463,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>319</v>
       </c>
@@ -4457,7 +4480,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>322</v>
       </c>
@@ -4474,7 +4497,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>325</v>
       </c>
@@ -4491,7 +4514,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>328</v>
       </c>
@@ -4508,7 +4531,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>331</v>
       </c>
@@ -4525,7 +4548,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>334</v>
       </c>
@@ -4542,7 +4565,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>337</v>
       </c>
@@ -4559,7 +4582,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>340</v>
       </c>
@@ -4578,7 +4601,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>343</v>
       </c>
@@ -4595,7 +4618,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>346</v>
       </c>
@@ -4612,7 +4635,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>349</v>
       </c>
@@ -4629,7 +4652,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>352</v>
       </c>
@@ -4646,7 +4669,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>355</v>
       </c>
@@ -4663,7 +4686,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>358</v>
       </c>
@@ -4680,7 +4703,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>361</v>
       </c>
@@ -4697,7 +4720,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>364</v>
       </c>
@@ -4714,7 +4737,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>367</v>
       </c>
@@ -4731,7 +4754,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>370</v>
       </c>
@@ -4750,7 +4773,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>373</v>
       </c>
@@ -4767,7 +4790,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>376</v>
       </c>
@@ -4784,7 +4807,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>380</v>
       </c>
@@ -4801,7 +4824,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>383</v>
       </c>
@@ -4818,7 +4841,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>386</v>
       </c>
@@ -4835,7 +4858,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>389</v>
       </c>
@@ -4849,7 +4872,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>391</v>
       </c>
@@ -4866,7 +4889,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>394</v>
       </c>
@@ -4883,7 +4906,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>397</v>
       </c>
@@ -4900,7 +4923,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>400</v>
       </c>
@@ -4917,7 +4940,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>403</v>
       </c>
@@ -4934,7 +4957,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>406</v>
       </c>
@@ -4954,7 +4977,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>409</v>
       </c>
@@ -4974,7 +4997,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>412</v>
       </c>
@@ -4991,7 +5014,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>415</v>
       </c>
@@ -5008,7 +5031,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>418</v>
       </c>
@@ -5025,7 +5048,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>421</v>
       </c>
@@ -5042,7 +5065,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>424</v>
       </c>
@@ -5059,7 +5082,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>427</v>
       </c>
@@ -5076,7 +5099,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>279</v>
       </c>
@@ -5093,7 +5116,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>432</v>
       </c>
@@ -5110,7 +5133,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>436</v>
       </c>
@@ -5127,7 +5150,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>439</v>
       </c>
@@ -5144,7 +5167,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>442</v>
       </c>
@@ -5161,7 +5184,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>445</v>
       </c>
@@ -5178,7 +5201,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>448</v>
       </c>
@@ -5195,7 +5218,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>451</v>
       </c>
@@ -5212,7 +5235,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>454</v>
       </c>
@@ -5229,7 +5252,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>457</v>
       </c>
@@ -5246,7 +5269,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>460</v>
       </c>
@@ -5263,7 +5286,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>463</v>
       </c>
@@ -5280,7 +5303,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>466</v>
       </c>
@@ -5297,7 +5320,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>469</v>
       </c>
@@ -5314,7 +5337,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>472</v>
       </c>
@@ -5331,7 +5354,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>475</v>
       </c>
@@ -5348,7 +5371,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>17</v>
       </c>
@@ -5365,7 +5388,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>480</v>
       </c>
@@ -5382,7 +5405,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>483</v>
       </c>
@@ -5399,7 +5422,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>487</v>
       </c>
@@ -5416,7 +5439,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>490</v>
       </c>
@@ -5433,7 +5456,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>493</v>
       </c>
@@ -5450,7 +5473,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>496</v>
       </c>
@@ -5467,7 +5490,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>499</v>
       </c>
@@ -5484,7 +5507,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>502</v>
       </c>
@@ -5501,7 +5524,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>505</v>
       </c>
@@ -5518,7 +5541,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>508</v>
       </c>
@@ -5535,7 +5558,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>511</v>
       </c>
@@ -5552,7 +5575,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>514</v>
       </c>
@@ -5569,7 +5592,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>517</v>
       </c>
@@ -5586,7 +5609,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>520</v>
       </c>
@@ -5603,7 +5626,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>523</v>
       </c>
@@ -5620,7 +5643,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>526</v>
       </c>
@@ -5637,7 +5660,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>529</v>
       </c>
@@ -5654,7 +5677,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>532</v>
       </c>
@@ -5671,7 +5694,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>535</v>
       </c>
@@ -5688,7 +5711,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>538</v>
       </c>
@@ -5705,7 +5728,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>541</v>
       </c>
@@ -5722,7 +5745,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>544</v>
       </c>
@@ -5739,7 +5762,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>547</v>
       </c>
@@ -5756,7 +5779,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>550</v>
       </c>
@@ -5773,7 +5796,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>553</v>
       </c>
@@ -5790,7 +5813,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>556</v>
       </c>
@@ -5807,7 +5830,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>560</v>
       </c>
@@ -5824,7 +5847,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>563</v>
       </c>
@@ -5841,7 +5864,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>566</v>
       </c>
@@ -5858,7 +5881,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>569</v>
       </c>
@@ -5872,7 +5895,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>571</v>
       </c>
@@ -5889,7 +5912,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>574</v>
       </c>
@@ -5906,7 +5929,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>577</v>
       </c>
@@ -5923,7 +5946,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>580</v>
       </c>
@@ -5940,7 +5963,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>583</v>
       </c>
@@ -5957,7 +5980,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>586</v>
       </c>
@@ -5974,7 +5997,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>589</v>
       </c>
@@ -5991,7 +6014,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>592</v>
       </c>
@@ -6008,7 +6031,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>595</v>
       </c>
@@ -6025,7 +6048,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>598</v>
       </c>
@@ -6042,7 +6065,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>601</v>
       </c>
@@ -6059,7 +6082,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>604</v>
       </c>
@@ -6076,7 +6099,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>607</v>
       </c>
@@ -6093,7 +6116,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>609</v>
       </c>
@@ -6107,7 +6130,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>611</v>
       </c>
@@ -6124,7 +6147,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>614</v>
       </c>
@@ -6141,7 +6164,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>617</v>
       </c>
@@ -6158,7 +6181,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>620</v>
       </c>
@@ -6175,7 +6198,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>623</v>
       </c>
@@ -6192,7 +6215,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>626</v>
       </c>
@@ -6209,7 +6232,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>630</v>
       </c>
@@ -6226,7 +6249,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>633</v>
       </c>
@@ -6243,7 +6266,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>636</v>
       </c>
@@ -6260,7 +6283,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>639</v>
       </c>
@@ -6277,7 +6300,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>642</v>
       </c>
@@ -6294,7 +6317,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>645</v>
       </c>
@@ -6311,7 +6334,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>648</v>
       </c>
@@ -6328,7 +6351,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>651</v>
       </c>
@@ -6345,7 +6368,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>654</v>
       </c>
@@ -6362,7 +6385,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>657</v>
       </c>
@@ -6379,7 +6402,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>660</v>
       </c>
@@ -6396,7 +6419,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>663</v>
       </c>
@@ -6413,7 +6436,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>666</v>
       </c>
@@ -6430,7 +6453,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>669</v>
       </c>
@@ -6447,7 +6470,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>672</v>
       </c>
@@ -6464,7 +6487,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>675</v>
       </c>
@@ -6481,7 +6504,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>678</v>
       </c>
@@ -6498,7 +6521,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>681</v>
       </c>
@@ -6515,7 +6538,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>684</v>
       </c>
@@ -6532,7 +6555,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>687</v>
       </c>
@@ -6549,7 +6572,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>691</v>
       </c>
@@ -6566,7 +6589,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>694</v>
       </c>
@@ -6583,7 +6606,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>697</v>
       </c>
@@ -6600,7 +6623,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>700</v>
       </c>
@@ -6618,6 +6641,24 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I227" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Consumo de agua potable y servicio de alcantarillado por habitante, por región (2022)"/>
+        <filter val="Consumo de energía por sector económico (2010/2023)"/>
+        <filter val="Consumo interno de materiales por tipo de material (2000-2024)"/>
+        <filter val="Consumo interno de materiales, y su relación al PIB y la población (2014-2024)"/>
+        <filter val="Consumo total de agua potable y recolección de aguas servidas residencial, por región (2022)"/>
+        <filter val="Consumo y Producción Sustentables"/>
+        <filter val="Dinámica del consumo de energía final en relación a la población a nivel nacional (2010-2024)"/>
+        <filter val="Evolución del consumo de agua continental en la minería del cobre, por proceso (2015-2024)"/>
+        <filter val="Evolución del consumo unitario de agua continental por tonelada de material procesado (2015-2024)"/>
+        <filter val="Participación de energéticos en el consumo del sector industrial y minero (Tcal) desagregado (2010-2023)"/>
+        <filter val="Participación de energéticos en el consumo del sector residencial, público, sanitario y comercial (Tcal) desagregado (2010-2023)"/>
+        <filter val="Participación de energéticos en el consumo del sector transporte (Tcal) desagregado (2010-2022)"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{1ADECD37-49C6-4485-8BA0-533803CCB521}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{121DC88B-2576-4E7C-8AC4-162549149903}"/>

</xml_diff>